<commit_message>
Generic Part location has been added for update in receive part tab
</commit_message>
<xml_diff>
--- a/files/templates/ERV.xlsx
+++ b/files/templates/ERV.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,7 +151,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-1009]d/mmm/yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-1009]d\-mmm\-yy;@"/>
@@ -842,24 +842,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -898,6 +880,24 @@
     </xf>
     <xf numFmtId="2" fontId="9" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="9" fillId="3" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1232,11 +1232,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1246,29 +1246,29 @@
     <col min="5" max="5" width="35.7109375" style="42" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="32" customWidth="1"/>
     <col min="7" max="7" width="17.7109375" style="26" customWidth="1"/>
-    <col min="8" max="8" width="42.7109375" style="36" customWidth="1"/>
-    <col min="9" max="9" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="51.85546875" style="36" customWidth="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
     <col min="10" max="10" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="21" thickBot="1">
-      <c r="A1" s="43"/>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="57"/>
+      <c r="B1" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="48"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
       <c r="F1" s="27"/>
       <c r="G1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50"/>
-      <c r="J1" s="51"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" spans="1:10" ht="15.75">
-      <c r="A2" s="44"/>
+      <c r="A2" s="58"/>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1281,12 +1281,12 @@
       <c r="G2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="54"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="48"/>
     </row>
     <row r="3" spans="1:10" ht="15.75">
-      <c r="A3" s="44"/>
+      <c r="A3" s="58"/>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1299,12 +1299,12 @@
       <c r="G3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="52"/>
-      <c r="I3" s="53"/>
-      <c r="J3" s="54"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
+      <c r="J3" s="48"/>
     </row>
     <row r="4" spans="1:10" ht="15.75">
-      <c r="A4" s="44"/>
+      <c r="A4" s="58"/>
       <c r="B4" s="4"/>
       <c r="C4" s="7"/>
       <c r="D4" s="6" t="s">
@@ -1313,12 +1313,12 @@
       <c r="E4" s="39"/>
       <c r="F4" s="28"/>
       <c r="G4" s="22"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="57"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
+      <c r="J4" s="51"/>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickBot="1">
-      <c r="A5" s="45"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="8"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10" t="s">
@@ -1327,9 +1327,9 @@
       <c r="E5" s="40"/>
       <c r="F5" s="29"/>
       <c r="G5" s="23"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="54"/>
     </row>
     <row r="6" spans="1:10" ht="16.5" thickBot="1">
       <c r="A6" s="11"/>
@@ -1343,15 +1343,15 @@
     </row>
     <row r="7" spans="1:10" ht="18.75" thickBot="1">
       <c r="A7" s="37"/>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="56"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
     </row>
     <row r="8" spans="1:10" ht="18" thickBot="1">
       <c r="A8" s="13" t="s">

</xml_diff>